<commit_message>
[BI-1158] update test and remove abbreviations from trait table
</commit_message>
<xml_diff>
--- a/src/test/resources/files/data_multiple_rows.xlsx
+++ b/src/test/resources/files/data_multiple_rows.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hms243-admin/IdeaProjects/bi-api/src/test/resources/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drp227/source/bi-api/src/test/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9EE23D2-B22B-0A4D-AD91-9A3C801F0BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117272C0-82B2-014B-80AD-D9968C3B47DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="32980" windowHeight="16800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,19 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
-  <si>
-    <t>Ontology term name</t>
-  </si>
-  <si>
-    <t>Trait abbreviations</t>
-  </si>
-  <si>
-    <t>Trait synonyms</t>
-  </si>
-  <si>
-    <t>Trait description</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>Trait entity</t>
   </si>
@@ -45,9 +33,6 @@
     <t>Trait attribute</t>
   </si>
   <si>
-    <t>Trait status</t>
-  </si>
-  <si>
     <t>Tags</t>
   </si>
   <si>
@@ -63,9 +48,6 @@
     <t>Method formula</t>
   </si>
   <si>
-    <t>Scale name</t>
-  </si>
-  <si>
     <t>Scale class</t>
   </si>
   <si>
@@ -84,9 +66,6 @@
     <t>Powdery Mildew severity field, leaves</t>
   </si>
   <si>
-    <t xml:space="preserve">PMSevLeaf; PM_LEAF_P4 </t>
-  </si>
-  <si>
     <t>Powdery Mildew Leaf; Powdery Mildew Severity Leaf</t>
   </si>
   <si>
@@ -129,9 +108,6 @@
     <t>Powdery Mildew severity field, bud</t>
   </si>
   <si>
-    <t xml:space="preserve">PMSevBud; PM_BUD_P4 </t>
-  </si>
-  <si>
     <t>Powdery Mildew Bud; Powdery Mildew Severity Bud</t>
   </si>
   <si>
@@ -144,9 +120,6 @@
     <t>Powdery Mildew severity field, stem</t>
   </si>
   <si>
-    <t xml:space="preserve">PMSevStem; PM_STEM_P4 </t>
-  </si>
-  <si>
     <t>Powdery Mildew Stem; Powdery Mildew Severity Stem</t>
   </si>
   <si>
@@ -166,6 +139,21 @@
   </si>
   <si>
     <t>Powdery Mildew Severity Stem</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Synonyms</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -517,246 +505,233 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="33.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="45.83203125" customWidth="1"/>
-    <col min="4" max="4" width="62.5" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" customWidth="1"/>
-    <col min="6" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="49.1640625" customWidth="1"/>
-    <col min="9" max="9" width="38.6640625" customWidth="1"/>
-    <col min="10" max="10" width="40.33203125" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="26.5" customWidth="1"/>
-    <col min="14" max="14" width="11" customWidth="1"/>
-    <col min="15" max="15" width="18.83203125" customWidth="1"/>
-    <col min="16" max="16" width="14.83203125" customWidth="1"/>
-    <col min="17" max="17" width="15" customWidth="1"/>
-    <col min="18" max="18" width="74" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" customWidth="1"/>
+    <col min="3" max="3" width="62.5" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="49.1640625" customWidth="1"/>
+    <col min="8" max="8" width="38.6640625" customWidth="1"/>
+    <col min="9" max="9" width="40.33203125" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="26.5" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="18.83203125" customWidth="1"/>
+    <col min="15" max="15" width="14.83203125" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
+    <col min="17" max="17" width="74" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
-        <v>43</v>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
+      <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="J3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
+      <c r="K3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
+      <c r="L3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
+      <c r="M3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" t="s">
-        <v>31</v>
-      </c>
-      <c r="R2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="S3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="S4" t="s">
-        <v>46</v>
+      <c r="Q4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[BI-1613] - Updating test files
</commit_message>
<xml_diff>
--- a/src/test/resources/files/data_multiple_rows.xlsx
+++ b/src/test/resources/files/data_multiple_rows.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drp227/source/bi-api/src/test/resources/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hms243/IdeaProjects/bi-api/src/test/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117272C0-82B2-014B-80AD-D9968C3B47DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6589B8FA-E774-8446-8FE8-A76D3D681070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32980" windowHeight="16800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1840" yWindow="4820" windowWidth="32980" windowHeight="16800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" refMode="R1C1"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>Trait entity</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Term Type</t>
+  </si>
+  <si>
+    <t>Germplasm Attribute</t>
+  </si>
+  <si>
+    <t>phenotype</t>
   </si>
 </sst>
 </file>
@@ -188,9 +197,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -531,7 +539,7 @@
     <col min="17" max="17" width="74" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -586,8 +594,11 @@
       <c r="R1" t="s">
         <v>34</v>
       </c>
+      <c r="S1" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -633,105 +644,105 @@
       <c r="R2" t="s">
         <v>35</v>
       </c>
+      <c r="S2" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>29</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" t="s">
         <v>25</v>
       </c>
       <c r="R3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>33</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" t="s">
         <v>24</v>
       </c>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" t="s">
         <v>25</v>
       </c>
       <c r="R4" t="s">
         <v>37</v>
+      </c>
+      <c r="S4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[BI-2053] - fixed tests
</commit_message>
<xml_diff>
--- a/src/test/resources/files/data_multiple_rows.xlsx
+++ b/src/test/resources/files/data_multiple_rows.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hms243/IdeaProjects/bi-api/src/test/resources/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mlm483/Source/bi-api/src/test/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6589B8FA-E774-8446-8FE8-A76D3D681070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE58168D-1E1F-3F44-8BAB-247B13276D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="4820" windowWidth="32980" windowHeight="16800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4860" yWindow="4820" windowWidth="32980" windowHeight="16800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Trait entity</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>a^2 + b^2 = c^2</t>
-  </si>
-  <si>
-    <t>1-4 Parlier field response score</t>
   </si>
   <si>
     <t>Ordinal</t>
@@ -515,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -541,13 +538,13 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>39</v>
-      </c>
-      <c r="C1" t="s">
-        <v>40</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -556,7 +553,7 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -574,7 +571,7 @@
         <v>6</v>
       </c>
       <c r="L1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M1" t="s">
         <v>7</v>
@@ -592,10 +589,10 @@
         <v>11</v>
       </c>
       <c r="R1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.15">
@@ -632,34 +629,31 @@
       <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" t="s">
-        <v>25</v>
-      </c>
       <c r="R2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -682,31 +676,28 @@
       <c r="K3" t="s">
         <v>22</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>23</v>
       </c>
-      <c r="M3" t="s">
+      <c r="Q3" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" t="s">
-        <v>25</v>
-      </c>
       <c r="R3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>33</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -729,20 +720,17 @@
       <c r="K4" t="s">
         <v>22</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>23</v>
       </c>
-      <c r="M4" t="s">
+      <c r="Q4" t="s">
         <v>24</v>
       </c>
-      <c r="Q4" t="s">
-        <v>25</v>
-      </c>
       <c r="R4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>